<commit_message>
Contains updated week numbers
</commit_message>
<xml_diff>
--- a/Documentation/Initial_planning_schedule.xlsx
+++ b/Documentation/Initial_planning_schedule.xlsx
@@ -18,9 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
-    <t>Week 14</t>
-  </si>
-  <si>
     <t>Week 15</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>Portuguese Class (Gavin)</t>
+  </si>
+  <si>
+    <t>Week 24</t>
   </si>
 </sst>
 </file>
@@ -500,7 +500,7 @@
   <dimension ref="A1:BS12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="BM3" sqref="BM3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +595,7 @@
       <c r="BK2" s="8"/>
       <c r="BL2" s="9"/>
       <c r="BM2" s="7" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="BN2" s="8"/>
       <c r="BO2" s="8"/>
@@ -818,13 +818,13 @@
     </row>
     <row r="5" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="5"/>
     </row>
     <row r="6" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="5"/>
@@ -841,7 +841,7 @@
     </row>
     <row r="7" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
@@ -860,7 +860,7 @@
     </row>
     <row r="8" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AB8" s="5"/>
       <c r="AC8" s="5"/>
@@ -893,7 +893,7 @@
     </row>
     <row r="9" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="BD9" s="5"/>
       <c r="BE9" s="5"/>
@@ -912,7 +912,7 @@
     </row>
     <row r="10" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="5"/>
@@ -935,7 +935,7 @@
     </row>
     <row r="11" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F11" s="5"/>
       <c r="M11" s="5"/>
@@ -951,7 +951,7 @@
     </row>
     <row r="12" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="5"/>
       <c r="J12" s="5"/>
@@ -966,16 +966,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AK2:AQ2"/>
+    <mergeCell ref="AR2:AX2"/>
+    <mergeCell ref="AY2:BE2"/>
+    <mergeCell ref="BF2:BL2"/>
+    <mergeCell ref="BM2:BS2"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="I2:O2"/>
     <mergeCell ref="P2:V2"/>
     <mergeCell ref="W2:AC2"/>
     <mergeCell ref="AD2:AJ2"/>
-    <mergeCell ref="AK2:AQ2"/>
-    <mergeCell ref="AR2:AX2"/>
-    <mergeCell ref="AY2:BE2"/>
-    <mergeCell ref="BF2:BL2"/>
-    <mergeCell ref="BM2:BS2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Formatted Schedule for PDF and updated PDF.
</commit_message>
<xml_diff>
--- a/Documentation/Initial_planning_schedule.xlsx
+++ b/Documentation/Initial_planning_schedule.xlsx
@@ -12,6 +12,10 @@
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$A$2:$H$13,Sheet1!$I$2:$O$13,Sheet1!$P$2:$V$13,Sheet1!$W$2:$AC$13,Sheet1!$AD$2:$AJ$14,Sheet1!$AK$2:$AQ$13,Sheet1!$AR$2:$AX$13,Sheet1!$AY$2:$BE$13,Sheet1!$BF$2:$BL$13,Sheet1!$BM$2:$BS$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Sheet1!$2:$13</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
@@ -191,7 +195,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -217,10 +221,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -299,13 +299,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
+    <tabColor rgb="FFFFFFFF"/>
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A2:BS13"/>
+  <dimension ref="A1:BS13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BM2" activeCellId="0" sqref="BM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -315,7 +315,81 @@
     <col collapsed="false" hidden="false" max="1025" min="72" style="1" width="8.6734693877551"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0"/>
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
+      <c r="L1" s="0"/>
+      <c r="M1" s="0"/>
+      <c r="N1" s="0"/>
+      <c r="O1" s="0"/>
+      <c r="P1" s="0"/>
+      <c r="Q1" s="0"/>
+      <c r="R1" s="0"/>
+      <c r="S1" s="0"/>
+      <c r="T1" s="0"/>
+      <c r="U1" s="0"/>
+      <c r="V1" s="0"/>
+      <c r="W1" s="0"/>
+      <c r="X1" s="0"/>
+      <c r="Y1" s="0"/>
+      <c r="Z1" s="0"/>
+      <c r="AA1" s="0"/>
+      <c r="AB1" s="0"/>
+      <c r="AC1" s="0"/>
+      <c r="AD1" s="0"/>
+      <c r="AE1" s="0"/>
+      <c r="AF1" s="0"/>
+      <c r="AG1" s="0"/>
+      <c r="AH1" s="0"/>
+      <c r="AI1" s="0"/>
+      <c r="AJ1" s="0"/>
+      <c r="AK1" s="0"/>
+      <c r="AL1" s="0"/>
+      <c r="AM1" s="0"/>
+      <c r="AN1" s="0"/>
+      <c r="AO1" s="0"/>
+      <c r="AP1" s="0"/>
+      <c r="AQ1" s="0"/>
+      <c r="AR1" s="0"/>
+      <c r="AS1" s="0"/>
+      <c r="AT1" s="0"/>
+      <c r="AU1" s="0"/>
+      <c r="AV1" s="0"/>
+      <c r="AW1" s="0"/>
+      <c r="AX1" s="0"/>
+      <c r="AY1" s="0"/>
+      <c r="AZ1" s="0"/>
+      <c r="BA1" s="0"/>
+      <c r="BB1" s="0"/>
+      <c r="BC1" s="0"/>
+      <c r="BD1" s="0"/>
+      <c r="BE1" s="0"/>
+      <c r="BF1" s="0"/>
+      <c r="BG1" s="0"/>
+      <c r="BH1" s="0"/>
+      <c r="BI1" s="0"/>
+      <c r="BJ1" s="0"/>
+      <c r="BK1" s="0"/>
+      <c r="BL1" s="0"/>
+      <c r="BM1" s="0"/>
+      <c r="BN1" s="0"/>
+      <c r="BO1" s="0"/>
+      <c r="BP1" s="0"/>
+      <c r="BQ1" s="0"/>
+      <c r="BR1" s="0"/>
+      <c r="BS1" s="0"/>
+    </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -408,6 +482,7 @@
       <c r="BS2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0"/>
       <c r="B3" s="3" t="n">
         <v>42401</v>
       </c>
@@ -618,18 +693,155 @@
       <c r="BS3" s="5" t="n">
         <v>42470</v>
       </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0"/>
+      <c r="B4" s="0"/>
+      <c r="C4" s="0"/>
+      <c r="D4" s="0"/>
+      <c r="E4" s="0"/>
+      <c r="F4" s="0"/>
+      <c r="G4" s="0"/>
+      <c r="H4" s="0"/>
+      <c r="I4" s="0"/>
+      <c r="J4" s="0"/>
+      <c r="K4" s="0"/>
+      <c r="L4" s="0"/>
+      <c r="M4" s="0"/>
+      <c r="N4" s="0"/>
+      <c r="O4" s="0"/>
+      <c r="P4" s="0"/>
+      <c r="Q4" s="0"/>
+      <c r="R4" s="0"/>
+      <c r="S4" s="0"/>
+      <c r="T4" s="0"/>
+      <c r="U4" s="0"/>
+      <c r="V4" s="0"/>
+      <c r="W4" s="0"/>
+      <c r="X4" s="0"/>
+      <c r="Y4" s="0"/>
+      <c r="Z4" s="0"/>
+      <c r="AA4" s="0"/>
+      <c r="AB4" s="0"/>
+      <c r="AC4" s="0"/>
+      <c r="AD4" s="0"/>
+      <c r="AE4" s="0"/>
+      <c r="AF4" s="0"/>
+      <c r="AG4" s="0"/>
+      <c r="AH4" s="0"/>
+      <c r="AI4" s="0"/>
+      <c r="AJ4" s="0"/>
+      <c r="AK4" s="0"/>
+      <c r="AL4" s="0"/>
+      <c r="AM4" s="0"/>
+      <c r="AN4" s="0"/>
+      <c r="AO4" s="0"/>
+      <c r="AP4" s="0"/>
+      <c r="AQ4" s="0"/>
+      <c r="AR4" s="0"/>
+      <c r="AS4" s="0"/>
+      <c r="AT4" s="0"/>
+      <c r="AU4" s="0"/>
+      <c r="AV4" s="0"/>
+      <c r="AW4" s="0"/>
+      <c r="AX4" s="0"/>
+      <c r="AY4" s="0"/>
+      <c r="AZ4" s="0"/>
+      <c r="BA4" s="0"/>
+      <c r="BB4" s="0"/>
+      <c r="BC4" s="0"/>
+      <c r="BD4" s="0"/>
+      <c r="BE4" s="0"/>
+      <c r="BF4" s="0"/>
+      <c r="BG4" s="0"/>
+      <c r="BH4" s="0"/>
+      <c r="BI4" s="0"/>
+      <c r="BJ4" s="0"/>
+      <c r="BK4" s="0"/>
+      <c r="BL4" s="0"/>
+      <c r="BM4" s="0"/>
+      <c r="BN4" s="0"/>
+      <c r="BO4" s="0"/>
+      <c r="BP4" s="0"/>
+      <c r="BQ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="6"/>
+      <c r="C5" s="0"/>
+      <c r="D5" s="0"/>
+      <c r="E5" s="0"/>
+      <c r="F5" s="0"/>
+      <c r="G5" s="0"/>
+      <c r="H5" s="0"/>
+      <c r="I5" s="0"/>
+      <c r="J5" s="0"/>
+      <c r="K5" s="0"/>
+      <c r="L5" s="0"/>
+      <c r="M5" s="0"/>
+      <c r="N5" s="0"/>
+      <c r="O5" s="0"/>
+      <c r="P5" s="0"/>
+      <c r="Q5" s="0"/>
+      <c r="R5" s="0"/>
+      <c r="S5" s="0"/>
+      <c r="T5" s="0"/>
+      <c r="U5" s="0"/>
+      <c r="V5" s="0"/>
+      <c r="W5" s="0"/>
+      <c r="X5" s="0"/>
+      <c r="Y5" s="0"/>
+      <c r="Z5" s="0"/>
+      <c r="AA5" s="0"/>
+      <c r="AB5" s="0"/>
+      <c r="AC5" s="0"/>
+      <c r="AD5" s="0"/>
+      <c r="AE5" s="0"/>
+      <c r="AF5" s="0"/>
+      <c r="AG5" s="0"/>
+      <c r="AH5" s="0"/>
+      <c r="AI5" s="0"/>
+      <c r="AJ5" s="0"/>
+      <c r="AK5" s="0"/>
+      <c r="AL5" s="0"/>
+      <c r="AM5" s="0"/>
+      <c r="AN5" s="0"/>
+      <c r="AO5" s="0"/>
+      <c r="AP5" s="0"/>
+      <c r="AQ5" s="0"/>
+      <c r="AR5" s="0"/>
+      <c r="AS5" s="0"/>
+      <c r="AT5" s="0"/>
+      <c r="AU5" s="0"/>
+      <c r="AV5" s="0"/>
+      <c r="AW5" s="0"/>
+      <c r="AX5" s="0"/>
+      <c r="AY5" s="0"/>
+      <c r="AZ5" s="0"/>
+      <c r="BA5" s="0"/>
+      <c r="BB5" s="0"/>
+      <c r="BC5" s="0"/>
+      <c r="BD5" s="0"/>
+      <c r="BE5" s="0"/>
+      <c r="BF5" s="0"/>
+      <c r="BG5" s="0"/>
+      <c r="BH5" s="0"/>
+      <c r="BI5" s="0"/>
+      <c r="BJ5" s="0"/>
+      <c r="BK5" s="0"/>
+      <c r="BL5" s="0"/>
+      <c r="BM5" s="0"/>
+      <c r="BN5" s="0"/>
+      <c r="BO5" s="0"/>
+      <c r="BP5" s="0"/>
+      <c r="BQ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="7"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -641,11 +853,75 @@
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
+      <c r="N6" s="0"/>
+      <c r="O6" s="0"/>
+      <c r="P6" s="0"/>
+      <c r="Q6" s="0"/>
+      <c r="R6" s="0"/>
+      <c r="S6" s="0"/>
+      <c r="T6" s="0"/>
+      <c r="U6" s="0"/>
+      <c r="V6" s="0"/>
+      <c r="W6" s="0"/>
+      <c r="X6" s="0"/>
+      <c r="Y6" s="0"/>
+      <c r="Z6" s="0"/>
+      <c r="AA6" s="0"/>
+      <c r="AB6" s="0"/>
+      <c r="AC6" s="0"/>
+      <c r="AD6" s="0"/>
+      <c r="AE6" s="0"/>
+      <c r="AF6" s="0"/>
+      <c r="AG6" s="0"/>
+      <c r="AH6" s="0"/>
+      <c r="AI6" s="0"/>
+      <c r="AJ6" s="0"/>
+      <c r="AK6" s="0"/>
+      <c r="AL6" s="0"/>
+      <c r="AM6" s="0"/>
+      <c r="AN6" s="0"/>
+      <c r="AO6" s="0"/>
+      <c r="AP6" s="0"/>
+      <c r="AQ6" s="0"/>
+      <c r="AR6" s="0"/>
+      <c r="AS6" s="0"/>
+      <c r="AT6" s="0"/>
+      <c r="AU6" s="0"/>
+      <c r="AV6" s="0"/>
+      <c r="AW6" s="0"/>
+      <c r="AX6" s="0"/>
+      <c r="AY6" s="0"/>
+      <c r="AZ6" s="0"/>
+      <c r="BA6" s="0"/>
+      <c r="BB6" s="0"/>
+      <c r="BC6" s="0"/>
+      <c r="BD6" s="0"/>
+      <c r="BE6" s="0"/>
+      <c r="BF6" s="0"/>
+      <c r="BG6" s="0"/>
+      <c r="BH6" s="0"/>
+      <c r="BI6" s="0"/>
+      <c r="BJ6" s="0"/>
+      <c r="BK6" s="0"/>
+      <c r="BL6" s="0"/>
+      <c r="BM6" s="0"/>
+      <c r="BN6" s="0"/>
+      <c r="BO6" s="0"/>
+      <c r="BP6" s="0"/>
+      <c r="BQ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C7" s="0"/>
+      <c r="D7" s="0"/>
+      <c r="E7" s="0"/>
+      <c r="F7" s="0"/>
+      <c r="J7" s="0"/>
+      <c r="K7" s="0"/>
+      <c r="L7" s="0"/>
+      <c r="M7" s="0"/>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
@@ -660,11 +936,68 @@
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
       <c r="AA7" s="6"/>
+      <c r="AB7" s="0"/>
+      <c r="AC7" s="0"/>
+      <c r="AD7" s="0"/>
+      <c r="AE7" s="0"/>
+      <c r="AF7" s="0"/>
+      <c r="AG7" s="0"/>
+      <c r="AH7" s="0"/>
+      <c r="AI7" s="0"/>
+      <c r="AJ7" s="0"/>
+      <c r="AK7" s="0"/>
+      <c r="AL7" s="0"/>
+      <c r="AM7" s="0"/>
+      <c r="AN7" s="0"/>
+      <c r="AO7" s="0"/>
+      <c r="AP7" s="0"/>
+      <c r="AQ7" s="0"/>
+      <c r="AR7" s="0"/>
+      <c r="AS7" s="0"/>
+      <c r="AT7" s="0"/>
+      <c r="AU7" s="0"/>
+      <c r="AV7" s="0"/>
+      <c r="AW7" s="0"/>
+      <c r="AX7" s="0"/>
+      <c r="AY7" s="0"/>
+      <c r="AZ7" s="0"/>
+      <c r="BA7" s="0"/>
+      <c r="BB7" s="0"/>
+      <c r="BC7" s="0"/>
+      <c r="BD7" s="0"/>
+      <c r="BE7" s="0"/>
+      <c r="BF7" s="0"/>
+      <c r="BG7" s="0"/>
+      <c r="BH7" s="0"/>
+      <c r="BI7" s="0"/>
+      <c r="BJ7" s="0"/>
+      <c r="BK7" s="0"/>
+      <c r="BL7" s="0"/>
+      <c r="BM7" s="0"/>
+      <c r="BN7" s="0"/>
+      <c r="BO7" s="0"/>
+      <c r="BP7" s="0"/>
+      <c r="BQ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
+      <c r="F8" s="0"/>
+      <c r="J8" s="0"/>
+      <c r="K8" s="0"/>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
+      <c r="Q8" s="0"/>
+      <c r="R8" s="0"/>
+      <c r="S8" s="0"/>
+      <c r="T8" s="0"/>
+      <c r="X8" s="0"/>
+      <c r="Z8" s="0"/>
+      <c r="AA8" s="0"/>
       <c r="AB8" s="6"/>
       <c r="AC8" s="6"/>
       <c r="AD8" s="6"/>
@@ -693,11 +1026,52 @@
       <c r="BA8" s="6"/>
       <c r="BB8" s="6"/>
       <c r="BC8" s="6"/>
+      <c r="BD8" s="0"/>
+      <c r="BE8" s="0"/>
+      <c r="BF8" s="0"/>
+      <c r="BG8" s="0"/>
+      <c r="BH8" s="0"/>
+      <c r="BI8" s="0"/>
+      <c r="BJ8" s="0"/>
+      <c r="BK8" s="0"/>
+      <c r="BL8" s="0"/>
+      <c r="BM8" s="0"/>
+      <c r="BN8" s="0"/>
+      <c r="BO8" s="0"/>
+      <c r="BP8" s="0"/>
+      <c r="BQ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C9" s="0"/>
+      <c r="D9" s="0"/>
+      <c r="E9" s="0"/>
+      <c r="F9" s="0"/>
+      <c r="J9" s="0"/>
+      <c r="K9" s="0"/>
+      <c r="L9" s="0"/>
+      <c r="M9" s="0"/>
+      <c r="Q9" s="0"/>
+      <c r="R9" s="0"/>
+      <c r="S9" s="0"/>
+      <c r="T9" s="0"/>
+      <c r="X9" s="0"/>
+      <c r="Z9" s="0"/>
+      <c r="AA9" s="0"/>
+      <c r="AE9" s="0"/>
+      <c r="AG9" s="0"/>
+      <c r="AH9" s="0"/>
+      <c r="AL9" s="0"/>
+      <c r="AN9" s="0"/>
+      <c r="AO9" s="0"/>
+      <c r="AS9" s="0"/>
+      <c r="AU9" s="0"/>
+      <c r="AV9" s="0"/>
+      <c r="AZ9" s="0"/>
+      <c r="BB9" s="0"/>
+      <c r="BC9" s="0"/>
       <c r="BD9" s="6"/>
       <c r="BE9" s="6"/>
       <c r="BF9" s="6"/>
@@ -717,39 +1091,56 @@
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="C10" s="0"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
-      <c r="K10" s="7"/>
+      <c r="J10" s="0"/>
       <c r="L10" s="6"/>
-      <c r="M10" s="7"/>
-      <c r="R10" s="7"/>
+      <c r="Q10" s="0"/>
       <c r="S10" s="6"/>
-      <c r="T10" s="7"/>
+      <c r="X10" s="0"/>
       <c r="Z10" s="6"/>
-      <c r="AA10" s="7"/>
+      <c r="AE10" s="0"/>
       <c r="AG10" s="6"/>
+      <c r="AH10" s="0"/>
+      <c r="AL10" s="0"/>
       <c r="AN10" s="6"/>
+      <c r="AO10" s="0"/>
+      <c r="AS10" s="0"/>
       <c r="AU10" s="6"/>
+      <c r="AV10" s="0"/>
+      <c r="AZ10" s="0"/>
       <c r="BB10" s="6"/>
+      <c r="BC10" s="0"/>
+      <c r="BG10" s="0"/>
       <c r="BI10" s="6"/>
-      <c r="BO10" s="7"/>
+      <c r="BJ10" s="0"/>
+      <c r="BN10" s="0"/>
       <c r="BP10" s="6"/>
+      <c r="BQ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="C11" s="0"/>
       <c r="F11" s="6"/>
+      <c r="J11" s="0"/>
       <c r="M11" s="6"/>
+      <c r="Q11" s="0"/>
       <c r="T11" s="6"/>
+      <c r="X11" s="0"/>
       <c r="AA11" s="6"/>
+      <c r="AE11" s="0"/>
       <c r="AH11" s="6"/>
+      <c r="AL11" s="0"/>
       <c r="AO11" s="6"/>
+      <c r="AS11" s="0"/>
       <c r="AV11" s="6"/>
+      <c r="AZ11" s="0"/>
       <c r="BC11" s="6"/>
+      <c r="BG11" s="0"/>
       <c r="BJ11" s="6"/>
-      <c r="BP11" s="7"/>
+      <c r="BN11" s="0"/>
       <c r="BQ11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -761,6 +1152,7 @@
       <c r="Q12" s="6"/>
       <c r="X12" s="6"/>
       <c r="AE12" s="6"/>
+      <c r="AH12" s="0"/>
       <c r="AL12" s="6"/>
       <c r="AS12" s="6"/>
       <c r="AZ12" s="6"/>
@@ -786,9 +1178,9 @@
     <mergeCell ref="BF2:BL2"/>
     <mergeCell ref="BM2:BS2"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="2" pageOrder="overThenDown" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -799,12 +1191,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -826,12 +1218,12 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>